<commit_message>
edited exc uni doc
</commit_message>
<xml_diff>
--- a/extra/POSSIBILI UNI PER ERASMUS.xlsx
+++ b/extra/POSSIBILI UNI PER ERASMUS.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EB89D0-8FF5-4380-9E9B-A521A6427D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411152F4-F30E-48AB-8C23-4E10B8CDEA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F68F9FDF-9B77-4370-99AD-20B158563E45}"/>
   </bookViews>
   <sheets>
     <sheet name="TUTTI I CORSI" sheetId="1" r:id="rId1"/>
     <sheet name="UNIVERSITA" sheetId="2" r:id="rId2"/>
-    <sheet name="Foglio1" sheetId="3" r:id="rId3"/>
+    <sheet name="rapporti richieste posti" sheetId="3" r:id="rId3"/>
+    <sheet name="Foglio2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="366">
   <si>
     <t>UNI</t>
   </si>
@@ -1130,6 +1131,12 @@
   </si>
   <si>
     <t>I corsi undergraduate sono soprattutto annuali. No TESI. I corsi vanno scelti all'interno di un solo Dipartimento.</t>
+  </si>
+  <si>
+    <t>uni</t>
+  </si>
+  <si>
+    <t>corsi possibili</t>
   </si>
 </sst>
 </file>
@@ -1387,7 +1394,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1402,10 +1409,6 @@
     <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -1462,6 +1465,10 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1888,7 +1895,7 @@
     <tableColumn id="4" xr3:uid="{F7D3BC16-7959-4617-9DDC-8866B07849B1}" name="Note" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{D65C89CA-B245-48D2-B3CE-C79EA9B8BCF6}" name="Posti Disponibili" dataDxfId="7"/>
     <tableColumn id="6" xr3:uid="{4E1B0D5C-BF71-4D73-A728-0C7897F3AA2F}" name="Candidature Bandi precedente a.a." dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{441EE02A-3AE6-4428-9C5F-B88EC916A99F}" name="rapporto" dataDxfId="0" dataCellStyle="Percentuale">
+    <tableColumn id="7" xr3:uid="{441EE02A-3AE6-4428-9C5F-B88EC916A99F}" name="rapporto" dataDxfId="5" dataCellStyle="Percentuale">
       <calculatedColumnFormula>E2/F2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4490,18 +4497,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1048576">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="2">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="IDK">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="IDK">
       <formula>NOT(ISERROR(SEARCH("IDK",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="KO">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="KO">
       <formula>NOT(ISERROR(SEARCH("KO",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5058,7 +5065,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A35">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5073,8 +5080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF90E40B-6F5B-46FE-A78E-7EB9B5156B53}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.44140625" defaultRowHeight="22.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5130,7 +5137,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="25">
-        <f>E2/F2</f>
+        <f t="shared" ref="G2:G33" si="0">E2/F2</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -5150,7 +5157,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="25">
-        <f>E3/F3</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
@@ -5172,7 +5179,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="25">
-        <f>E4/F4</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
@@ -5194,7 +5201,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="25">
-        <f>E5/F5</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
@@ -5216,7 +5223,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="25">
-        <f>E6/F6</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -5238,7 +5245,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="25">
-        <f>E7/F7</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -5262,7 +5269,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="25">
-        <f>E8/F8</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -5282,7 +5289,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="25">
-        <f>E9/F9</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -5302,7 +5309,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="25">
-        <f>E10/F10</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -5326,7 +5333,7 @@
         <v>7</v>
       </c>
       <c r="G11" s="25">
-        <f>E11/F11</f>
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
     </row>
@@ -5346,7 +5353,7 @@
         <v>14</v>
       </c>
       <c r="G12" s="25">
-        <f>E12/F12</f>
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
     </row>
@@ -5370,7 +5377,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="25">
-        <f>E13/F13</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
@@ -5392,7 +5399,7 @@
         <v>4</v>
       </c>
       <c r="G14" s="25">
-        <f>E14/F14</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
@@ -5414,7 +5421,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="25">
-        <f>E15/F15</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
@@ -5436,7 +5443,7 @@
         <v>8</v>
       </c>
       <c r="G16" s="25">
-        <f>E16/F16</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
@@ -5458,7 +5465,7 @@
         <v>12</v>
       </c>
       <c r="G17" s="25">
-        <f>E17/F17</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
@@ -5482,7 +5489,7 @@
         <v>14</v>
       </c>
       <c r="G18" s="25">
-        <f>E18/F18</f>
+        <f t="shared" si="0"/>
         <v>0.21428571428571427</v>
       </c>
     </row>
@@ -5504,7 +5511,7 @@
         <v>5</v>
       </c>
       <c r="G19" s="25">
-        <f>E19/F19</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -5526,7 +5533,7 @@
         <v>5</v>
       </c>
       <c r="G20" s="25">
-        <f>E20/F20</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -5548,7 +5555,7 @@
         <v>5</v>
       </c>
       <c r="G21" s="25">
-        <f>E21/F21</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -5570,7 +5577,7 @@
         <v>10</v>
       </c>
       <c r="G22" s="25">
-        <f>E22/F22</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -5592,7 +5599,7 @@
         <v>10</v>
       </c>
       <c r="G23" s="25">
-        <f>E23/F23</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -5614,7 +5621,7 @@
         <v>11</v>
       </c>
       <c r="G24" s="25">
-        <f>E24/F24</f>
+        <f t="shared" si="0"/>
         <v>0.18181818181818182</v>
       </c>
     </row>
@@ -5636,7 +5643,7 @@
         <v>11</v>
       </c>
       <c r="G25" s="25">
-        <f>E25/F25</f>
+        <f t="shared" si="0"/>
         <v>0.18181818181818182</v>
       </c>
     </row>
@@ -5658,7 +5665,7 @@
         <v>12</v>
       </c>
       <c r="G26" s="25">
-        <f>E26/F26</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -5680,7 +5687,7 @@
         <v>24</v>
       </c>
       <c r="G27" s="25">
-        <f>E27/F27</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -5702,7 +5709,7 @@
         <v>13</v>
       </c>
       <c r="G28" s="25">
-        <f>E28/F28</f>
+        <f t="shared" si="0"/>
         <v>0.15384615384615385</v>
       </c>
     </row>
@@ -5724,7 +5731,7 @@
         <v>7</v>
       </c>
       <c r="G29" s="25">
-        <f>E29/F29</f>
+        <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -5748,7 +5755,7 @@
         <v>15</v>
       </c>
       <c r="G30" s="25">
-        <f>E30/F30</f>
+        <f t="shared" si="0"/>
         <v>0.13333333333333333</v>
       </c>
     </row>
@@ -5772,7 +5779,7 @@
         <v>8</v>
       </c>
       <c r="G31" s="25">
-        <f>E31/F31</f>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
     </row>
@@ -5794,7 +5801,7 @@
         <v>16</v>
       </c>
       <c r="G32" s="25">
-        <f>E32/F32</f>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
     </row>
@@ -5818,7 +5825,7 @@
         <v>32</v>
       </c>
       <c r="G33" s="25">
-        <f>E33/F33</f>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
     </row>
@@ -5838,7 +5845,7 @@
         <v>101</v>
       </c>
       <c r="G34" s="25">
-        <f>E34/F34</f>
+        <f t="shared" ref="G34:G65" si="1">E34/F34</f>
         <v>0.11881188118811881</v>
       </c>
     </row>
@@ -5860,7 +5867,7 @@
         <v>26</v>
       </c>
       <c r="G35" s="25">
-        <f>E35/F35</f>
+        <f t="shared" si="1"/>
         <v>0.11538461538461539</v>
       </c>
     </row>
@@ -5882,7 +5889,7 @@
         <v>18</v>
       </c>
       <c r="G36" s="25">
-        <f>E36/F36</f>
+        <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
@@ -5904,7 +5911,7 @@
         <v>18</v>
       </c>
       <c r="G37" s="25">
-        <f>E37/F37</f>
+        <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
@@ -5926,7 +5933,7 @@
         <v>46</v>
       </c>
       <c r="G38" s="25">
-        <f>E38/F38</f>
+        <f t="shared" si="1"/>
         <v>0.10869565217391304</v>
       </c>
     </row>
@@ -5948,7 +5955,7 @@
         <v>19</v>
       </c>
       <c r="G39" s="25">
-        <f>E39/F39</f>
+        <f t="shared" si="1"/>
         <v>0.10526315789473684</v>
       </c>
     </row>
@@ -5972,7 +5979,7 @@
         <v>19</v>
       </c>
       <c r="G40" s="25">
-        <f>E40/F40</f>
+        <f t="shared" si="1"/>
         <v>0.10526315789473684</v>
       </c>
     </row>
@@ -5994,7 +6001,7 @@
         <v>19</v>
       </c>
       <c r="G41" s="25">
-        <f>E41/F41</f>
+        <f t="shared" si="1"/>
         <v>0.10526315789473684</v>
       </c>
     </row>
@@ -6016,7 +6023,7 @@
         <v>29</v>
       </c>
       <c r="G42" s="25">
-        <f>E42/F42</f>
+        <f t="shared" si="1"/>
         <v>0.10344827586206896</v>
       </c>
     </row>
@@ -6038,7 +6045,7 @@
         <v>22</v>
       </c>
       <c r="G43" s="25">
-        <f>E43/F43</f>
+        <f t="shared" si="1"/>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
@@ -6060,7 +6067,7 @@
         <v>34</v>
       </c>
       <c r="G44" s="25">
-        <f>E44/F44</f>
+        <f t="shared" si="1"/>
         <v>8.8235294117647065E-2</v>
       </c>
     </row>
@@ -6080,7 +6087,7 @@
         <v>34</v>
       </c>
       <c r="G45" s="25">
-        <f>E45/F45</f>
+        <f t="shared" si="1"/>
         <v>8.8235294117647065E-2</v>
       </c>
     </row>
@@ -6104,7 +6111,7 @@
         <v>23</v>
       </c>
       <c r="G46" s="25">
-        <f>E46/F46</f>
+        <f t="shared" si="1"/>
         <v>8.6956521739130432E-2</v>
       </c>
     </row>
@@ -6128,7 +6135,7 @@
         <v>71</v>
       </c>
       <c r="G47" s="25">
-        <f>E47/F47</f>
+        <f t="shared" si="1"/>
         <v>8.4507042253521125E-2</v>
       </c>
     </row>
@@ -6148,7 +6155,7 @@
         <v>24</v>
       </c>
       <c r="G48" s="25">
-        <f>E48/F48</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
@@ -6172,7 +6179,7 @@
         <v>37</v>
       </c>
       <c r="G49" s="25">
-        <f>E49/F49</f>
+        <f t="shared" si="1"/>
         <v>8.1081081081081086E-2</v>
       </c>
     </row>
@@ -6194,7 +6201,7 @@
         <v>27</v>
       </c>
       <c r="G50" s="25">
-        <f>E50/F50</f>
+        <f t="shared" si="1"/>
         <v>7.407407407407407E-2</v>
       </c>
     </row>
@@ -6216,7 +6223,7 @@
         <v>14</v>
       </c>
       <c r="G51" s="25">
-        <f>E51/F51</f>
+        <f t="shared" si="1"/>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
@@ -6238,7 +6245,7 @@
         <v>112</v>
       </c>
       <c r="G52" s="25">
-        <f>E52/F52</f>
+        <f t="shared" si="1"/>
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
@@ -6258,7 +6265,7 @@
         <v>29</v>
       </c>
       <c r="G53" s="25">
-        <f>E53/F53</f>
+        <f t="shared" si="1"/>
         <v>6.8965517241379309E-2</v>
       </c>
     </row>
@@ -6278,7 +6285,7 @@
         <v>61</v>
       </c>
       <c r="G54" s="25">
-        <f>E54/F54</f>
+        <f t="shared" si="1"/>
         <v>6.5573770491803282E-2</v>
       </c>
     </row>
@@ -6298,7 +6305,7 @@
         <v>46</v>
       </c>
       <c r="G55" s="25">
-        <f>E55/F55</f>
+        <f t="shared" si="1"/>
         <v>6.5217391304347824E-2</v>
       </c>
     </row>
@@ -6322,7 +6329,7 @@
         <v>31</v>
       </c>
       <c r="G56" s="25">
-        <f>E56/F56</f>
+        <f t="shared" si="1"/>
         <v>6.4516129032258063E-2</v>
       </c>
     </row>
@@ -6342,7 +6349,7 @@
         <v>47</v>
       </c>
       <c r="G57" s="25">
-        <f>E57/F57</f>
+        <f t="shared" si="1"/>
         <v>6.3829787234042548E-2</v>
       </c>
     </row>
@@ -6364,7 +6371,7 @@
         <v>34</v>
       </c>
       <c r="G58" s="25">
-        <f>E58/F58</f>
+        <f t="shared" si="1"/>
         <v>5.8823529411764705E-2</v>
       </c>
     </row>
@@ -6386,7 +6393,7 @@
         <v>34</v>
       </c>
       <c r="G59" s="25">
-        <f>E59/F59</f>
+        <f t="shared" si="1"/>
         <v>5.8823529411764705E-2</v>
       </c>
     </row>
@@ -6408,7 +6415,7 @@
         <v>53</v>
       </c>
       <c r="G60" s="25">
-        <f>E60/F60</f>
+        <f t="shared" si="1"/>
         <v>5.6603773584905662E-2</v>
       </c>
     </row>
@@ -6430,7 +6437,7 @@
         <v>71</v>
       </c>
       <c r="G61" s="25">
-        <f>E61/F61</f>
+        <f t="shared" si="1"/>
         <v>5.6338028169014086E-2</v>
       </c>
     </row>
@@ -6454,7 +6461,7 @@
         <v>78</v>
       </c>
       <c r="G62" s="25">
-        <f>E62/F62</f>
+        <f t="shared" si="1"/>
         <v>5.128205128205128E-2</v>
       </c>
     </row>
@@ -6476,7 +6483,7 @@
         <v>20</v>
       </c>
       <c r="G63" s="25">
-        <f>E63/F63</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
     </row>
@@ -6496,7 +6503,7 @@
         <v>40</v>
       </c>
       <c r="G64" s="25">
-        <f>E64/F64</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
     </row>
@@ -6520,7 +6527,7 @@
         <v>129</v>
       </c>
       <c r="G65" s="25">
-        <f>E65/F65</f>
+        <f t="shared" si="1"/>
         <v>4.6511627906976744E-2</v>
       </c>
     </row>
@@ -6540,7 +6547,7 @@
         <v>45</v>
       </c>
       <c r="G66" s="25">
-        <f>E66/F66</f>
+        <f t="shared" ref="G66:G97" si="2">E66/F66</f>
         <v>4.4444444444444446E-2</v>
       </c>
     </row>
@@ -6562,7 +6569,7 @@
         <v>92</v>
       </c>
       <c r="G67" s="25">
-        <f>E67/F67</f>
+        <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
@@ -6584,7 +6591,7 @@
         <v>46</v>
       </c>
       <c r="G68" s="25">
-        <f>E68/F68</f>
+        <f t="shared" si="2"/>
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
@@ -6606,7 +6613,7 @@
         <v>117</v>
       </c>
       <c r="G69" s="25">
-        <f>E69/F69</f>
+        <f t="shared" si="2"/>
         <v>4.2735042735042736E-2</v>
       </c>
     </row>
@@ -6630,7 +6637,7 @@
         <v>95</v>
       </c>
       <c r="G70" s="25">
-        <f>E70/F70</f>
+        <f t="shared" si="2"/>
         <v>4.2105263157894736E-2</v>
       </c>
     </row>
@@ -6652,7 +6659,7 @@
         <v>172</v>
       </c>
       <c r="G71" s="25">
-        <f>E71/F71</f>
+        <f t="shared" si="2"/>
         <v>4.0697674418604654E-2</v>
       </c>
     </row>
@@ -6676,7 +6683,7 @@
         <v>74</v>
       </c>
       <c r="G72" s="25">
-        <f>E72/F72</f>
+        <f t="shared" si="2"/>
         <v>4.0540540540540543E-2</v>
       </c>
     </row>
@@ -6698,7 +6705,7 @@
         <v>100</v>
       </c>
       <c r="G73" s="25">
-        <f>E73/F73</f>
+        <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
     </row>
@@ -6720,7 +6727,7 @@
         <v>27</v>
       </c>
       <c r="G74" s="25">
-        <f>E74/F74</f>
+        <f t="shared" si="2"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -6742,7 +6749,7 @@
         <v>81</v>
       </c>
       <c r="G75" s="25">
-        <f>E75/F75</f>
+        <f t="shared" si="2"/>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
@@ -6766,7 +6773,7 @@
         <v>28</v>
       </c>
       <c r="G76" s="25">
-        <f>E76/F76</f>
+        <f t="shared" si="2"/>
         <v>3.5714285714285712E-2</v>
       </c>
     </row>
@@ -6788,7 +6795,7 @@
         <v>60</v>
       </c>
       <c r="G77" s="25">
-        <f>E77/F77</f>
+        <f t="shared" si="2"/>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
@@ -6810,7 +6817,7 @@
         <v>90</v>
       </c>
       <c r="G78" s="25">
-        <f>E78/F78</f>
+        <f t="shared" si="2"/>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
@@ -6830,7 +6837,7 @@
         <v>64</v>
       </c>
       <c r="G79" s="25">
-        <f>E79/F79</f>
+        <f t="shared" si="2"/>
         <v>3.125E-2</v>
       </c>
     </row>
@@ -6854,7 +6861,7 @@
         <v>36</v>
       </c>
       <c r="G80" s="25">
-        <f>E80/F80</f>
+        <f t="shared" si="2"/>
         <v>2.7777777777777776E-2</v>
       </c>
     </row>
@@ -6876,7 +6883,7 @@
         <v>151</v>
       </c>
       <c r="G81" s="25">
-        <f>E81/F81</f>
+        <f t="shared" si="2"/>
         <v>2.6490066225165563E-2</v>
       </c>
     </row>
@@ -6896,7 +6903,7 @@
         <v>164</v>
       </c>
       <c r="G82" s="25">
-        <f>E82/F82</f>
+        <f t="shared" si="2"/>
         <v>2.4390243902439025E-2</v>
       </c>
     </row>
@@ -6920,7 +6927,7 @@
         <v>206</v>
       </c>
       <c r="G83" s="25">
-        <f>E83/F83</f>
+        <f t="shared" si="2"/>
         <v>2.4271844660194174E-2</v>
       </c>
     </row>
@@ -6942,7 +6949,7 @@
         <v>130</v>
       </c>
       <c r="G84" s="25">
-        <f>E84/F84</f>
+        <f t="shared" si="2"/>
         <v>2.3076923076923078E-2</v>
       </c>
     </row>
@@ -6964,7 +6971,7 @@
         <v>141</v>
       </c>
       <c r="G85" s="25">
-        <f>E85/F85</f>
+        <f t="shared" si="2"/>
         <v>2.1276595744680851E-2</v>
       </c>
     </row>
@@ -6986,7 +6993,7 @@
         <v>144</v>
       </c>
       <c r="G86" s="25">
-        <f>E86/F86</f>
+        <f t="shared" si="2"/>
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
@@ -7006,7 +7013,7 @@
         <v>79</v>
       </c>
       <c r="G87" s="25">
-        <f>E87/F87</f>
+        <f t="shared" si="2"/>
         <v>1.2658227848101266E-2</v>
       </c>
     </row>
@@ -7028,7 +7035,7 @@
         <v>164</v>
       </c>
       <c r="G88" s="25">
-        <f>E88/F88</f>
+        <f t="shared" si="2"/>
         <v>1.2195121951219513E-2</v>
       </c>
     </row>
@@ -7052,7 +7059,7 @@
         <v>85</v>
       </c>
       <c r="G89" s="25">
-        <f>E89/F89</f>
+        <f t="shared" si="2"/>
         <v>1.1764705882352941E-2</v>
       </c>
     </row>
@@ -7072,7 +7079,7 @@
         <v>300</v>
       </c>
       <c r="G90" s="25">
-        <f>E90/F90</f>
+        <f t="shared" si="2"/>
         <v>6.6666666666666671E-3</v>
       </c>
     </row>
@@ -7096,7 +7103,7 @@
         <v>180</v>
       </c>
       <c r="G91" s="25">
-        <f>E91/F91</f>
+        <f t="shared" si="2"/>
         <v>5.5555555555555558E-3</v>
       </c>
     </row>
@@ -7106,4 +7113,36 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E706027-A5A9-4425-A8A6-EF894AC7FD8A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
edited erasmus unis doc
</commit_message>
<xml_diff>
--- a/extra/POSSIBILI UNI PER ERASMUS.xlsx
+++ b/extra/POSSIBILI UNI PER ERASMUS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96586D38-11AC-4694-BAE8-C184E35F8B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B9BCEB-E68C-4146-AD8A-1B36F44D8637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F68F9FDF-9B77-4370-99AD-20B158563E45}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="384">
   <si>
     <t>UNI</t>
   </si>
@@ -1176,6 +1176,9 @@
   </si>
   <si>
     <t>TUTTI  I CORSI IN INGLESE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1488,15 @@
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
     <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -1947,7 +1958,7 @@
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{3AB1737B-AE5D-428E-9DD3-97B426C7EABE}"/>
     <tableStyle name="Stile tabella 1" pivot="0" count="1" xr9:uid="{58C5260B-747E-4936-8F34-F82861092E31}">
-      <tableStyleElement type="wholeTable" dxfId="21"/>
+      <tableStyleElement type="wholeTable" dxfId="22"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1969,7 +1980,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A2B8D22-03AC-4A0D-8ADB-F05C0671D6E9}" name="Tabella1" displayName="Tabella1" ref="A1:E35" totalsRowShown="0" headerRowBorderDxfId="20" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A2B8D22-03AC-4A0D-8ADB-F05C0671D6E9}" name="Tabella1" displayName="Tabella1" ref="A1:E35" totalsRowShown="0" headerRowBorderDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="A1:E35" xr:uid="{7A2B8D22-03AC-4A0D-8ADB-F05C0671D6E9}">
     <filterColumn colId="3">
       <filters>
@@ -1992,10 +2003,10 @@
     <sortCondition descending="1" ref="B1:B35"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5540347C-6B15-4327-8EDE-1678D98847FF}" name="UNI" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{3CBFBE6D-616C-4A1E-9263-F8704FFB844B}" name="CREDITI OK" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{238C71E2-371D-45B2-85A8-40B9A4A3BEE6}" name="CREDITI IDK" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{BF482025-BF83-4F60-87AC-A65BFF144610}" name="CREDITI OK + IDK" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{5540347C-6B15-4327-8EDE-1678D98847FF}" name="UNI" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{3CBFBE6D-616C-4A1E-9263-F8704FFB844B}" name="CREDITI OK" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{238C71E2-371D-45B2-85A8-40B9A4A3BEE6}" name="CREDITI IDK" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{BF482025-BF83-4F60-87AC-A65BFF144610}" name="CREDITI OK + IDK" dataDxfId="16">
       <calculatedColumnFormula>SUM(B2:C2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{ACF6EBFF-BA22-4328-AC9E-5C22F07538A1}" name="POSTI"/>
@@ -2005,22 +2016,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F526BFF-E58F-4150-9348-5F6184A80886}" name="Tabella3" displayName="Tabella3" ref="A1:H91" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:H91" xr:uid="{4F526BFF-E58F-4150-9348-5F6184A80886}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F526BFF-E58F-4150-9348-5F6184A80886}" name="Tabella3" displayName="Tabella3" ref="A1:H91" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:H91" xr:uid="{4F526BFF-E58F-4150-9348-5F6184A80886}">
+    <filterColumn colId="7">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H91">
     <sortCondition descending="1" ref="G1:G91"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{FB7EDB6B-A938-44B1-87FA-7B22971E8EDA}" name="Codice Ateneo" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{1D693904-57AB-4A81-BFA5-C2366BC0752D}" name="Nome Ateneo" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{BF004504-1CD4-4FC2-B321-4EC27CD6190B}" name="Struttura ospitante" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{F7D3BC16-7959-4617-9DDC-8866B07849B1}" name="Note" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{D65C89CA-B245-48D2-B3CE-C79EA9B8BCF6}" name="Posti Disponibili" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{4E1B0D5C-BF71-4D73-A728-0C7897F3AA2F}" name="Candidature Bandi precedente a.a." dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{441EE02A-3AE6-4428-9C5F-B88EC916A99F}" name="rapporto" dataDxfId="6" dataCellStyle="Percentuale">
+    <tableColumn id="1" xr3:uid="{FB7EDB6B-A938-44B1-87FA-7B22971E8EDA}" name="Codice Ateneo" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{1D693904-57AB-4A81-BFA5-C2366BC0752D}" name="Nome Ateneo" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{BF004504-1CD4-4FC2-B321-4EC27CD6190B}" name="Struttura ospitante" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{F7D3BC16-7959-4617-9DDC-8866B07849B1}" name="Note" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{D65C89CA-B245-48D2-B3CE-C79EA9B8BCF6}" name="Posti Disponibili" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{4E1B0D5C-BF71-4D73-A728-0C7897F3AA2F}" name="Candidature Bandi precedente a.a." dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{441EE02A-3AE6-4428-9C5F-B88EC916A99F}" name="rapporto" dataDxfId="7" dataCellStyle="Percentuale">
       <calculatedColumnFormula>E2/F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{9D45C25F-A487-4339-9DAA-1705A923AAE6}" name="esito controllo" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{9D45C25F-A487-4339-9DAA-1705A923AAE6}" name="esito controllo" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4620,18 +4635,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1048576">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="2">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="IDK">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="IDK">
       <formula>NOT(ISERROR(SEARCH("IDK",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="KO">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="KO">
       <formula>NOT(ISERROR(SEARCH("KO",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5188,7 +5203,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A35">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5201,15 +5216,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF90E40B-6F5B-46FE-A78E-7EB9B5156B53}">
-  <dimension ref="A1:H91"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="22.9" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="33.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" style="2"/>
@@ -5270,77 +5285,77 @@
         <v>365</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24">
-        <v>2</v>
-      </c>
-      <c r="F3" s="24">
-        <v>5</v>
+    <row r="3" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26">
+        <v>4</v>
+      </c>
+      <c r="F3" s="26">
+        <v>10</v>
       </c>
       <c r="G3" s="22">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="H3" s="30" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="29" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>175</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C4" s="24"/>
       <c r="D4" s="24"/>
       <c r="E4" s="24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4" s="24">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G4" s="22">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="H4" s="31" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26">
+      <c r="H4" s="30" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24">
         <v>4</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="24">
         <v>10</v>
       </c>
       <c r="G5" s="22">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="H5" s="29" t="s">
-        <v>367</v>
+      <c r="H5" s="31" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
@@ -5368,7 +5383,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>154</v>
       </c>
@@ -5393,7 +5408,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>157</v>
       </c>
@@ -5420,7 +5435,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>190</v>
       </c>
@@ -5439,11 +5454,11 @@
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="30" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>345</v>
       </c>
@@ -5468,52 +5483,52 @@
     </row>
     <row r="11" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>161</v>
+        <v>200</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>163</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F11" s="24">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G11" s="22">
         <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="H11" s="31" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="29" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="19.899999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>200</v>
+        <v>161</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
+        <v>93</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>163</v>
+      </c>
       <c r="E12" s="24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F12" s="24">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G12" s="22">
         <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="H12" s="29" t="s">
-        <v>371</v>
+      <c r="H12" s="31" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -5543,7 +5558,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>137</v>
       </c>
@@ -5568,7 +5583,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>140</v>
       </c>
@@ -5593,7 +5608,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="63.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>166</v>
       </c>
@@ -5618,7 +5633,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>192</v>
       </c>
@@ -5643,7 +5658,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>202</v>
       </c>
@@ -5696,56 +5711,56 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24">
+      <c r="A20" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26">
         <v>1</v>
       </c>
-      <c r="F20" s="24">
+      <c r="F20" s="26">
         <v>5</v>
       </c>
       <c r="G20" s="22">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="H20" s="31" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26">
+      <c r="H20" s="29" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24">
         <v>1</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="24">
         <v>5</v>
       </c>
       <c r="G21" s="22">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="H21" s="29" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="31" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>179</v>
       </c>
@@ -5770,7 +5785,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>181</v>
       </c>
@@ -5820,7 +5835,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>187</v>
       </c>
@@ -5843,7 +5858,7 @@
       </c>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>195</v>
       </c>
@@ -5866,7 +5881,7 @@
       </c>
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>237</v>
       </c>
@@ -5889,7 +5904,7 @@
       </c>
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>197</v>
       </c>
@@ -5912,7 +5927,7 @@
       </c>
       <c r="H28" s="27"/>
     </row>
-    <row r="29" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>164</v>
       </c>
@@ -5935,7 +5950,7 @@
       </c>
       <c r="H29" s="27"/>
     </row>
-    <row r="30" spans="1:8" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="105.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>209</v>
       </c>
@@ -5960,7 +5975,7 @@
       </c>
       <c r="H30" s="27"/>
     </row>
-    <row r="31" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>169</v>
       </c>
@@ -5985,7 +6000,7 @@
       </c>
       <c r="H31" s="27"/>
     </row>
-    <row r="32" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
         <v>213</v>
       </c>
@@ -6008,7 +6023,7 @@
       </c>
       <c r="H32" s="27"/>
     </row>
-    <row r="33" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>260</v>
       </c>
@@ -6033,7 +6048,7 @@
       </c>
       <c r="H33" s="27"/>
     </row>
-    <row r="34" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>320</v>
       </c>
@@ -6054,7 +6069,7 @@
       </c>
       <c r="H34" s="27"/>
     </row>
-    <row r="35" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>242</v>
       </c>
@@ -6077,7 +6092,7 @@
       </c>
       <c r="H35" s="27"/>
     </row>
-    <row r="36" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>215</v>
       </c>
@@ -6100,7 +6115,7 @@
       </c>
       <c r="H36" s="27"/>
     </row>
-    <row r="37" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
         <v>218</v>
       </c>
@@ -6123,7 +6138,7 @@
       </c>
       <c r="H37" s="27"/>
     </row>
-    <row r="38" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>277</v>
       </c>
@@ -6146,7 +6161,7 @@
       </c>
       <c r="H38" s="27"/>
     </row>
-    <row r="39" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>221</v>
       </c>
@@ -6169,7 +6184,7 @@
       </c>
       <c r="H39" s="27"/>
     </row>
-    <row r="40" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="44.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>224</v>
       </c>
@@ -6194,7 +6209,7 @@
       </c>
       <c r="H40" s="27"/>
     </row>
-    <row r="41" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>226</v>
       </c>
@@ -6217,7 +6232,7 @@
       </c>
       <c r="H41" s="27"/>
     </row>
-    <row r="42" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>251</v>
       </c>
@@ -6240,7 +6255,7 @@
       </c>
       <c r="H42" s="27"/>
     </row>
-    <row r="43" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>231</v>
       </c>
@@ -6263,7 +6278,7 @@
       </c>
       <c r="H43" s="27"/>
     </row>
-    <row r="44" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>263</v>
       </c>
@@ -6286,7 +6301,7 @@
       </c>
       <c r="H44" s="27"/>
     </row>
-    <row r="45" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>266</v>
       </c>
@@ -6307,7 +6322,7 @@
       </c>
       <c r="H45" s="27"/>
     </row>
-    <row r="46" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>233</v>
       </c>
@@ -6332,7 +6347,7 @@
       </c>
       <c r="H46" s="27"/>
     </row>
-    <row r="47" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
         <v>291</v>
       </c>
@@ -6357,7 +6372,7 @@
       </c>
       <c r="H47" s="27"/>
     </row>
-    <row r="48" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="23" t="s">
         <v>240</v>
       </c>
@@ -6378,7 +6393,7 @@
       </c>
       <c r="H48" s="27"/>
     </row>
-    <row r="49" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>209</v>
       </c>
@@ -6403,7 +6418,7 @@
       </c>
       <c r="H49" s="27"/>
     </row>
-    <row r="50" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
         <v>245</v>
       </c>
@@ -6426,7 +6441,7 @@
       </c>
       <c r="H50" s="27"/>
     </row>
-    <row r="51" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
         <v>206</v>
       </c>
@@ -6449,7 +6464,7 @@
       </c>
       <c r="H51" s="27"/>
     </row>
-    <row r="52" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
         <v>301</v>
       </c>
@@ -6472,7 +6487,7 @@
       </c>
       <c r="H52" s="27"/>
     </row>
-    <row r="53" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
         <v>254</v>
       </c>
@@ -6493,7 +6508,7 @@
       </c>
       <c r="H53" s="27"/>
     </row>
-    <row r="54" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
         <v>287</v>
       </c>
@@ -6514,7 +6529,7 @@
       </c>
       <c r="H54" s="27"/>
     </row>
-    <row r="55" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="25" t="s">
         <v>280</v>
       </c>
@@ -6535,7 +6550,7 @@
       </c>
       <c r="H55" s="27"/>
     </row>
-    <row r="56" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="23" t="s">
         <v>256</v>
       </c>
@@ -6560,7 +6575,7 @@
       </c>
       <c r="H56" s="27"/>
     </row>
-    <row r="57" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="23" t="s">
         <v>351</v>
       </c>
@@ -6581,7 +6596,7 @@
       </c>
       <c r="H57" s="27"/>
     </row>
-    <row r="58" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
         <v>267</v>
       </c>
@@ -6604,7 +6619,7 @@
       </c>
       <c r="H58" s="27"/>
     </row>
-    <row r="59" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="25" t="s">
         <v>270</v>
       </c>
@@ -6627,7 +6642,7 @@
       </c>
       <c r="H59" s="27"/>
     </row>
-    <row r="60" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="23" t="s">
         <v>282</v>
       </c>
@@ -6650,7 +6665,7 @@
       </c>
       <c r="H60" s="27"/>
     </row>
-    <row r="61" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="25" t="s">
         <v>294</v>
       </c>
@@ -6673,7 +6688,7 @@
       </c>
       <c r="H61" s="27"/>
     </row>
-    <row r="62" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
         <v>301</v>
       </c>
@@ -6698,7 +6713,7 @@
       </c>
       <c r="H62" s="27"/>
     </row>
-    <row r="63" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="23" t="s">
         <v>228</v>
       </c>
@@ -6721,7 +6736,7 @@
       </c>
       <c r="H63" s="27"/>
     </row>
-    <row r="64" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="23" t="s">
         <v>352</v>
       </c>
@@ -6742,7 +6757,7 @@
       </c>
       <c r="H64" s="27"/>
     </row>
-    <row r="65" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="23" t="s">
         <v>324</v>
       </c>
@@ -6767,7 +6782,7 @@
       </c>
       <c r="H65" s="27"/>
     </row>
-    <row r="66" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="25" t="s">
         <v>275</v>
       </c>
@@ -6783,12 +6798,12 @@
         <v>45</v>
       </c>
       <c r="G66" s="22">
-        <f t="shared" ref="G66:G91" si="2">E66/F66</f>
+        <f t="shared" ref="G66:G97" si="2">E66/F66</f>
         <v>4.4444444444444446E-2</v>
       </c>
       <c r="H66" s="27"/>
     </row>
-    <row r="67" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="23" t="s">
         <v>311</v>
       </c>
@@ -6811,7 +6826,7 @@
       </c>
       <c r="H67" s="27"/>
     </row>
-    <row r="68" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="23" t="s">
         <v>358</v>
       </c>
@@ -6834,7 +6849,7 @@
       </c>
       <c r="H68" s="27"/>
     </row>
-    <row r="69" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="25" t="s">
         <v>301</v>
       </c>
@@ -6857,7 +6872,7 @@
       </c>
       <c r="H69" s="27"/>
     </row>
-    <row r="70" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="25" t="s">
         <v>313</v>
       </c>
@@ -6882,7 +6897,7 @@
       </c>
       <c r="H70" s="27"/>
     </row>
-    <row r="71" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="25" t="s">
         <v>291</v>
       </c>
@@ -6905,7 +6920,7 @@
       </c>
       <c r="H71" s="27"/>
     </row>
-    <row r="72" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="23" t="s">
         <v>297</v>
       </c>
@@ -6930,7 +6945,7 @@
       </c>
       <c r="H72" s="27"/>
     </row>
-    <row r="73" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="23" t="s">
         <v>317</v>
       </c>
@@ -6953,7 +6968,7 @@
       </c>
       <c r="H73" s="27"/>
     </row>
-    <row r="74" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="25" t="s">
         <v>248</v>
       </c>
@@ -6976,7 +6991,7 @@
       </c>
       <c r="H74" s="27"/>
     </row>
-    <row r="75" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="25" t="s">
         <v>285</v>
       </c>
@@ -6999,7 +7014,7 @@
       </c>
       <c r="H75" s="27"/>
     </row>
-    <row r="76" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="23" t="s">
         <v>361</v>
       </c>
@@ -7024,7 +7039,7 @@
       </c>
       <c r="H76" s="27"/>
     </row>
-    <row r="77" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="25" t="s">
         <v>285</v>
       </c>
@@ -7047,7 +7062,7 @@
       </c>
       <c r="H77" s="27"/>
     </row>
-    <row r="78" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="25" t="s">
         <v>213</v>
       </c>
@@ -7070,7 +7085,7 @@
       </c>
       <c r="H78" s="27"/>
     </row>
-    <row r="79" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="36.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="25" t="s">
         <v>289</v>
       </c>
@@ -7091,7 +7106,7 @@
       </c>
       <c r="H79" s="27"/>
     </row>
-    <row r="80" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="23" t="s">
         <v>354</v>
       </c>
@@ -7116,7 +7131,7 @@
       </c>
       <c r="H80" s="27"/>
     </row>
-    <row r="81" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="23" t="s">
         <v>349</v>
       </c>
@@ -7139,7 +7154,7 @@
       </c>
       <c r="H81" s="27"/>
     </row>
-    <row r="82" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="25" t="s">
         <v>332</v>
       </c>
@@ -7160,7 +7175,7 @@
       </c>
       <c r="H82" s="27"/>
     </row>
-    <row r="83" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="44.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="25" t="s">
         <v>224</v>
       </c>
@@ -7185,7 +7200,7 @@
       </c>
       <c r="H83" s="27"/>
     </row>
-    <row r="84" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="20" t="s">
         <v>327</v>
       </c>
@@ -7208,7 +7223,7 @@
       </c>
       <c r="H84" s="27"/>
     </row>
-    <row r="85" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="23" t="s">
         <v>347</v>
       </c>
@@ -7231,7 +7246,7 @@
       </c>
       <c r="H85" s="27"/>
     </row>
-    <row r="86" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="23" t="s">
         <v>330</v>
       </c>
@@ -7254,7 +7269,7 @@
       </c>
       <c r="H86" s="27"/>
     </row>
-    <row r="87" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="23" t="s">
         <v>303</v>
       </c>
@@ -7275,7 +7290,7 @@
       </c>
       <c r="H87" s="27"/>
     </row>
-    <row r="88" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="23" t="s">
         <v>334</v>
       </c>
@@ -7298,7 +7313,7 @@
       </c>
       <c r="H88" s="27"/>
     </row>
-    <row r="89" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="23" t="s">
         <v>306</v>
       </c>
@@ -7323,7 +7338,7 @@
       </c>
       <c r="H89" s="27"/>
     </row>
-    <row r="90" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="22.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="23" t="s">
         <v>342</v>
       </c>
@@ -7344,7 +7359,7 @@
       </c>
       <c r="H90" s="27"/>
     </row>
-    <row r="91" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="23" t="s">
         <v>338</v>
       </c>
@@ -7368,6 +7383,11 @@
         <v>5.5555555555555558E-3</v>
       </c>
       <c r="H91" s="27"/>
+    </row>
+    <row r="94" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C94" s="2" t="s">
+        <v>383</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>